<commit_message>
add POC on loop in gherkin
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/hello.xlsx
+++ b/src/test/resources/data/out/hello.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="24">
   <si>
     <t>Résultat</t>
   </si>
@@ -96,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +122,21 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -297,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -338,6 +353,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,7 +713,7 @@
       <c r="E2" s="12">
         <v>43846</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="40" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="3"/>
@@ -714,7 +732,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="41" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="3"/>
@@ -733,7 +751,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="10"/>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="41" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="4"/>
@@ -752,7 +770,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="40" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3"/>
@@ -771,7 +789,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="41" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP WIP WIP WIP Use Chainable waits + test @AsPageElement Starting to refactor wait steps + all steps using a pageElement argument WIP WIP Reworked WaitSteps Reworked steps and put some to deprecated
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/hello.xlsx
+++ b/src/test/resources/data/out/hello.xlsx
@@ -2,18 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="NoraUi-hello" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NoraUi-hello" r:id="rId2" sheetId="1" state="visible"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Motifs" vbProcedure="false">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="34">
   <si>
     <t xml:space="preserve">author</t>
   </si>
@@ -95,6 +95,36 @@
   </si>
   <si>
     <t xml:space="preserve">Jenkins T8</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>This is a demo for NORAUI (Non-Regression Automation for User Interfaces).</t>
+  </si>
+  <si>
+    <t>Fail: The city is Paris!!</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Typing Â« Input Select field Â» in bakery. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ The value of the field Â« -input_current_date Â» is not the expected one (0) in bakery. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ The provided data Â« city Â» cannot be empty. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ The provided data Â« element Â» cannot be empty. /!\, /!\ The provided data Â« element2 Â» cannot be empty. /!\.</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Unable to authenticate with provided credentials. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Error on text data. The provided date must be greater than or equal to today. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Element not found on the page. /!\</t>
   </si>
 </sst>
 </file>
@@ -106,7 +136,7 @@
     <numFmt numFmtId="165" formatCode="[$-40C]DD/MM/YYYY"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="49">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -148,6 +178,216 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
   </fonts>
   <fills count="5">
@@ -177,7 +417,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -186,83 +426,125 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="53">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="35" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="36" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="38" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="40" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="41" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="42" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="43" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="44" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="45" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" name="Percent" xfId="19"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -332,21 +614,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I9" activeCellId="0" pane="topLeft" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.28"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="17.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="20.57" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="7" customWidth="true" hidden="false" style="0" width="15.57" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="16.28" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -372,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -391,11 +673,15 @@
       <c r="F2" s="5" t="n">
         <v>43846</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>32</v>
+      </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
@@ -413,12 +699,12 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="9" t="n">
-        <v>31</v>
+      <c r="H3" s="51" t="s">
+        <v>26</v>
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -436,12 +722,12 @@
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="9" t="n">
-        <v>25</v>
+      <c r="H4" s="51" t="s">
+        <v>27</v>
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -458,11 +744,15 @@
         <v>11</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>24</v>
+      </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
@@ -480,11 +770,11 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="9" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -500,11 +790,11 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
@@ -518,11 +808,11 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
@@ -538,138 +828,138 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="9" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="4"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Improved page toString + javadoc
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/hello.xlsx
+++ b/src/test/resources/data/out/hello.xlsx
@@ -2,18 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="NoraUi-hello" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NoraUi-hello" r:id="rId2" sheetId="1" state="visible"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Motifs" vbProcedure="false">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="37">
   <si>
     <t xml:space="preserve">author</t>
   </si>
@@ -95,6 +95,45 @@
   </si>
   <si>
     <t xml:space="preserve">Jenkins T8</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Fail: The city is Paris!!</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Typing Â« Input Select field Â» in bakery. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ The provided data Â« city Â» cannot be empty. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ The provided data Â« element Â» cannot be empty. /!\, /!\ The provided data Â« element2 Â» cannot be empty. /!\.</t>
+  </si>
+  <si>
+    <t>Fail: /!\ The value of the field Â« -input_current_date Â» is not the expected one (0) in bakery. /!\</t>
+  </si>
+  <si>
+    <t>This is a demo for NORAUI (Non-Regression Automation for User Interfaces).</t>
+  </si>
+  <si>
+    <t>{"total_count":229,"incomplete_results":false,"items":[{"login":"ndeloof","id":132757,"node_id":"MDQ6VXNlcjEzMjc1Nw==","avatar_url":"https://avatars0.githubusercontent.com/u/132757?v=4","gravatar_id":"","url":"https://api.github.com/users/ndeloof","html_url":"https://github.com/ndeloof","followers_url":"https://api.github.com/users/ndeloof/followers","following_url":"https://api.github.com/users/ndeloof/following{/other_user}","gists_url":"https://api.github.com/users/ndeloof/gists{/gist_id}","starred_url":"https://api.github.com/users/ndeloof/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/ndeloof/subscriptions","organizations_url":"https://api.github.com/users/ndeloof/orgs","repos_url":"https://api.github.com/users/ndeloof/repos","events_url":"https://api.github.com/users/ndeloof/events{/privacy}","received_events_url":"https://api.github.com/users/ndeloof/received_events","type":"User","site_admin":false,"score":1.0},{"login":"aurelhubert","id":4895410,"node_id":"MDQ6VXNlcjQ4OTU0MTA=","avatar_url":"https://avatars0.githubusercontent.com/u/4895410?v=4","gravatar_id":"","url":"https://api.github.com/users/aurelhubert","html_url":"https://github.com/aurelhubert","followers_url":"https://api.github.com/users/aurelhubert/followers","following_url":"https://api.github.com/users/aurelhubert/following{/other_user}","gists_url":"https://api.github.com/users/aurelhubert/gists{/gist_id}","starred_url":"https://api.github.com/users/aurelhubert/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/aurelhubert/subscriptions","organizations_url":"https://api.github.com/users/aurelhubert/orgs","repos_url":"https://api.github.com/users/aurelhubert/repos","events_url":"https://api.github.com/users/aurelhubert/events{/privacy}","received_events_url":"https://api.github.com/users/aurelhubert/received_events","type":"User","site_admin":false,"score":1.0},{"login":"pcmanus","id":479957,"node_id":"MDQ6VXNlcjQ3OTk1Nw==","avatar_url":"https://avatars3.githubusercontent.com/u/479957?v=4","gravatar_id":"","url":"https://api.github.com/users/pcmanus","html_url":"https://github.com/pcmanus","followers_url":"https://api.github.com/users/pcmanus/followers","following_url":"https://api.github.com/users/pcmanus/following{/other_user}","gists_url":"https://api.github.com/users/pcmanus/gists{/gist_id}","starred_url":"https://api.github.com/users/pcmanus/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/pcmanus/subscriptions","organizations_url":"https://api.github.com/users/pcmanus/orgs","repos_url":"https://api.github.com/users/pcmanus/repos","events_url":"https://api.github.com/users/pcmanus/events{/privacy}","received_events_url":"https://api.github.com/users/pcmanus/received_events","type":"User","site_admin":false,"score":1.0},{"login":"deruelle","id":54279,"node_id":"MDQ6VXNlcjU0Mjc5","avatar_url":"https://avatars3.githubusercontent.com/u/54279?v=4","gravatar_id":"","url":"https://api.github.com/users/deruelle","html_url":"https://github.com/deruelle","followers_url":"https://api.github.com/users/deruelle/followers","following_url":"https://api.github.com/users/deruelle/following{/other_user}","gists_url":"https://api.github.com/users/deruelle/gists{/gist_id}","starred_url":"https://api.github.com/users/deruelle/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/deruelle/subscriptions","organizations_url":"https://api.github.com/users/deruelle/orgs","repos_url":"https://api.github.com/users/deruelle/repos","events_url":"https://api.github.com/users/deruelle/events{/privacy}","received_events_url":"https://api.github.com/users/deruelle/received_events","type":"User","site_admin":false,"score":1.0},{"login":"barais","id":598311,"node_id":"MDQ6VXNlcjU5ODMxMQ==","avatar_url":"https://avatars1.githubusercontent.com/u/598311?v=4","gravatar_id":"","url":"https://api.github.com/users/barais","html_url":"https://github.com/barais","followers_url":"https://api.github.com/users/barais/followers","following_url":"https://api.github.com/users/barais/following{/other_user}","gists_url":"https://api.github.com/users/barais/gists{/gist_id}","starred_url":"https://api.github.com/users/barais/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/barais/subscriptions","organizations_url":"https://api.github.com/users/barais/orgs","repos_url":"https://api.github.com/users/barais/repos","events_url":"https://api.github.com/users/barais/events{/privacy}","received_events_url":"https://api.github.com/users/barais/received_events","type":"User","site_admin":false,"score":1.0},{"login":"ybonnel","id":428232,"node_id":"MDQ6VXNlcjQyODIzMg==","avatar_url":"https://avatars1.githubusercontent.com/u/428232?v=4","gravatar_id":"","url":"https://api.github.com/users/ybonnel","html_url":"https://github.com/ybonnel","followers_url":"https://api.github.com/users/ybonnel/followers","following_url":"https://api.github.com/users/ybonnel/following{/other_user}","gists_url":"https://api.github.com/users/ybonnel/gists{/gist_id}","starred_url":"https://api.github.com/users/ybonnel/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/ybonnel/subscriptions","organizations_url":"https://api.github.com/users/ybonnel/orgs","repos_url":"https://api.github.com/users/ybonnel/repos","events_url":"https://api.github.com/users/ybonnel/events{/privacy}","received_events_url":"https://api.github.com/users/ybonnel/received_events","type":"User","site_admin":false,"score":1.0},{"login":"ganfra","id":8754928,"node_id":"MDQ6VXNlcjg3NTQ5Mjg=","avatar_url":"https://avatars3.githubusercontent.com/u/8754928?v=4","gravatar_id":"","url":"https://api.github.com/users/ganfra","html_url":"https://github.com/ganfra","followers_url":"https://api.github.com/users/ganfra/followers","following_url":"https://api.github.com/users/ganfra/following{/other_user}","gists_url":"https://api.github.com/users/ganfra/gists{/gist_id}","starred_url":"https://api.github.com/users/ganfra/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/ganfra/subscriptions","organizations_url":"https://api.github.com/users/ganfra/orgs","repos_url":"https://api.github.com/users/ganfra/repos","events_url":"https://api.github.com/users/ganfra/events{/privacy}","received_events_url":"https://api.github.com/users/ganfra/received_events","type":"User","site_admin":false,"score":1.0},{"login":"Jean-Emile","id":1098811,"node_id":"MDQ6VXNlcjEwOTg4MTE=","avatar_url":"https://avatars3.githubusercontent.com/u/1098811?v=4","gravatar_id":"","url":"https://api.github.com/users/Jean-Emile","html_url":"https://github.com/Jean-Emile","followers_url":"https://api.github.com/users/Jean-Emile/followers","following_url":"https://api.github.com/users/Jean-Emile/following{/other_user}","gists_url":"https://api.github.com/users/Jean-Emile/gists{/gist_id}","starred_url":"https://api.github.com/users/Jean-Emile/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/Jean-Emile/subscriptions","organizations_url":"https://api.github.com/users/Jean-Emile/orgs","repos_url":"https://api.github.com/users/Jean-Emile/repos","events_url":"https://api.github.com/users/Jean-Emile/events{/privacy}","received_events_url":"https://api.github.com/users/Jean-Emile/received_events","type":"User","site_admin":false,"score":1.0},{"login":"arnobl","id":1052622,"node_id":"MDQ6VXNlcjEwNTI2MjI=","avatar_url":"https://avatars0.githubusercontent.com/u/1052622?v=4","gravatar_id":"","url":"https://api.github.com/users/arnobl","html_url":"https://github.com/arnobl","followers_url":"https://api.github.com/users/arnobl/followers","following_url":"https://api.github.com/users/arnobl/following{/other_user}","gists_url":"https://api.github.com/users/arnobl/gists{/gist_id}","starred_url":"https://api.github.com/users/arnobl/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/arnobl/subscriptions","organizations_url":"https://api.github.com/users/arnobl/orgs","repos_url":"https://api.github.com/users/arnobl/repos","events_url":"https://api.github.com/users/arnobl/events{/privacy}","received_events_url":"https://api.github.com/users/arnobl/received_events","type":"User","site_admin":false,"score":1.0},{"login":"acherm","id":530573,"node_id":"MDQ6VXNlcjUzMDU3Mw==","avatar_url":"https://avatars1.githubusercontent.com/u/530573?v=4","gravatar_id":"","url":"https://api.github.com/users/acherm","html_url":"https://github.com/acherm","followers_url":"https://api.github.com/users/acherm/followers","following_url":"https://api.github.com/users/acherm/following{/other_user}","gists_url":"https://api.github.com/users/acherm/gists{/gist_id}","starred_url":"https://api.github.com/users/acherm/starred{/owner}{/repo}","subscriptions_url":"https://api.github.com/users/acherm/subscriptions","organizations_url":"https://api.github.com/users/acherm/orgs","repos_url":"https://api.github.com/users/acherm/repos","events_url":"https://api.github.com/users/acherm/events{/privacy}","received_events_url":"https://api.github.com/users/acherm/received_events","type":"User","site_admin":false,"score":1.0}]}</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Click on Â« no exist element Â» in bakery. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ No value for Â« Input Text field Â» in bakery. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Typing Â« bakery.BAKERY_DEMO.Input Select field Â» in bakery. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Click on Â« bakery.BAKERY_DEMO.no exist element Â» in bakery. /!\</t>
+  </si>
+  <si>
+    <t>Fail: /!\ No value for Â« bakery.BAKERY_DEMO.Input Text field Â» in bakery. /!\</t>
   </si>
 </sst>
 </file>
@@ -106,7 +145,7 @@
     <numFmt numFmtId="165" formatCode="[$-40C]dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -148,6 +187,81 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
   </fonts>
   <fills count="5">
@@ -177,7 +291,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -186,79 +300,94 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="25">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" name="Percent" xfId="19"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -328,21 +457,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F2" activeCellId="0" pane="topLeft" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.28"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="17.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="20.57" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="7" customWidth="true" hidden="false" style="0" width="15.57" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="16.28" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -387,10 +516,14 @@
       <c r="F2" s="5" t="n">
         <v>54804</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -408,11 +541,11 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="8" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -430,12 +563,12 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="8" t="n">
-        <v>25</v>
+      <c r="H4" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -452,10 +585,14 @@
         <v>11</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
@@ -473,11 +610,11 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="8" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -493,11 +630,11 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
@@ -511,11 +648,11 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="8" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -530,139 +667,141 @@
         <v>11</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="40">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="41">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="44">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="45">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="46">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="A47" s="4"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fixed Page type cucumber regex
</commit_message>
<xml_diff>
--- a/src/test/resources/data/out/hello.xlsx
+++ b/src/test/resources/data/out/hello.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="37">
   <si>
     <t xml:space="preserve">author</t>
   </si>
@@ -145,7 +145,7 @@
     <numFmt numFmtId="165" formatCode="[$-40C]dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -187,6 +187,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -324,7 +339,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -377,9 +392,12 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -519,7 +537,7 @@
       <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="25" t="s">
         <v>24</v>
       </c>
     </row>
@@ -541,7 +559,7 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="26" t="s">
         <v>25</v>
       </c>
     </row>
@@ -563,7 +581,7 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="26" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="9"/>
@@ -588,7 +606,7 @@
       <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="25" t="s">
         <v>24</v>
       </c>
     </row>
@@ -610,7 +628,7 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="26" t="s">
         <v>35</v>
       </c>
     </row>
@@ -630,7 +648,7 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="26" t="s">
         <v>27</v>
       </c>
     </row>
@@ -648,7 +666,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -670,7 +688,7 @@
       <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="26" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>